<commit_message>
Improved documentation, new pic
</commit_message>
<xml_diff>
--- a/ProjectDependencies.xlsx
+++ b/ProjectDependencies.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\Infrastruktur\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\onetime\hrrno_web\hrr\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17592" windowHeight="5592"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17592" windowHeight="5592" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dependencies" sheetId="1" r:id="rId1"/>
     <sheet name="Specified dependencies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -98,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,13 +144,28 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -166,18 +180,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -187,38 +219,172 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </left>
       <right/>
       <top/>
@@ -228,7 +394,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </right>
       <top/>
       <bottom/>
@@ -236,12 +402,12 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -250,29 +416,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -280,97 +435,144 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,133 +854,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="7" width="9.21875" customWidth="1"/>
+    <col min="3" max="8" width="9.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="30" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="11" t="s">
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="G2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="17"/>
-    </row>
-    <row r="4" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="C4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
+      <c r="C6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="21"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="28"/>
-      <c r="G7" s="29"/>
+      <c r="C7" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="22"/>
+      <c r="E7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="C1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -787,137 +1094,228 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="6" width="25" customWidth="1"/>
-    <col min="7" max="7" width="28.44140625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="1"/>
+    <col min="3" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="10"/>
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="17"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="32.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" ht="32.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+    </row>
+    <row r="4" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="17"/>
+      <c r="B4" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="F4" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H4" s="34" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+    </row>
+    <row r="5" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="17"/>
+      <c r="B5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="C5" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="36"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="C6" s="37"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+    </row>
+    <row r="7" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="5" t="s">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H7" s="39" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:11" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F8" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>